<commit_message>
Calibration update and additional CB scens
Model with updated calibration, potentials update and new carbon budget scenarios,
small fixes and cleaning
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
+++ b/SubRES_TMPL/SubRES_TRA_NewVehicles.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bcf850925e8c42cd/Desktop/times-ireland-model/SubRES_TMPL/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VEDA\Veda_models\times-ireland-model-main\SubRES_TMPL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="228" documentId="13_ncr:1_{B81FD6BF-416C-4328-A15F-C59C43468514}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C952D0FF-535D-45BF-B84B-1C06F73728FC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{940EBF4A-B20D-4004-B94E-587CC3C959FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2656,9 +2656,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2696,9 +2696,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2731,26 +2731,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2783,26 +2766,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7144,8 +7110,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B3:X298"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E138" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T164" sqref="T164"/>
+    <sheetView tabSelected="1" topLeftCell="A226" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E251" sqref="E251"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -16856,7 +16822,7 @@
         <v>UP</v>
       </c>
       <c r="E249" s="62">
-        <v>0.95903634682608185</v>
+        <v>1</v>
       </c>
       <c r="F249" s="62">
         <v>1</v>
@@ -16908,10 +16874,11 @@
         <v>UP</v>
       </c>
       <c r="E251" s="62">
-        <v>0.5</v>
+        <v>0.95</v>
       </c>
       <c r="F251" s="62">
-        <v>0.5</v>
+        <f>E251</f>
+        <v>0.95</v>
       </c>
       <c r="G251" s="62">
         <v>1</v>
@@ -16934,10 +16901,12 @@
         <v>LO</v>
       </c>
       <c r="E252" s="62">
-        <v>0.5</v>
+        <f>E251</f>
+        <v>0.95</v>
       </c>
       <c r="F252" s="62">
-        <v>0.5</v>
+        <f>F251</f>
+        <v>0.95</v>
       </c>
       <c r="G252" s="62">
         <v>0</v>

</xml_diff>